<commit_message>
Getting through Z tray readout
</commit_message>
<xml_diff>
--- a/Active Projects/Work Z-tray Readout.xlsx
+++ b/Active Projects/Work Z-tray Readout.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="744">
   <si>
     <t>LED'S</t>
   </si>
@@ -1334,12 +1334,21 @@
     <t>ZT2326</t>
   </si>
   <si>
-    <t>ZT2400</t>
+    <t>zt2400</t>
   </si>
   <si>
     <t>ZT2465</t>
   </si>
   <si>
+    <t>zv1505</t>
+  </si>
+  <si>
+    <t>zv1515</t>
+  </si>
+  <si>
+    <t>zv1535</t>
+  </si>
+  <si>
     <t>ZV1564</t>
   </si>
   <si>
@@ -1349,13 +1358,16 @@
     <t>ZV1638</t>
   </si>
   <si>
-    <t>ZV1670</t>
+    <t>zv1646</t>
+  </si>
+  <si>
+    <t>zv1676</t>
   </si>
   <si>
     <t>ZC4009</t>
   </si>
   <si>
-    <t>ZC4016</t>
+    <t>zc4016</t>
   </si>
   <si>
     <t>ZC4020</t>
@@ -1394,13 +1406,79 @@
     <t>ZC4834</t>
   </si>
   <si>
+    <t>zt2287</t>
+  </si>
+  <si>
+    <t>zt2293</t>
+  </si>
+  <si>
+    <t>zt2300</t>
+  </si>
+  <si>
+    <t>zt2328</t>
+  </si>
+  <si>
+    <t>zt2450</t>
+  </si>
+  <si>
+    <t>zt2466</t>
+  </si>
+  <si>
+    <t>zv1506</t>
+  </si>
+  <si>
+    <t>zv1524</t>
+  </si>
+  <si>
+    <t>zv1539</t>
+  </si>
+  <si>
+    <t>zv1565</t>
+  </si>
+  <si>
+    <t>zv1634</t>
+  </si>
+  <si>
+    <t>zv1640</t>
+  </si>
+  <si>
+    <t>zv1650</t>
+  </si>
+  <si>
+    <t>zv1680</t>
+  </si>
+  <si>
+    <t>zc4011</t>
+  </si>
+  <si>
+    <t>zc4017</t>
+  </si>
+  <si>
+    <t>zc4023</t>
+  </si>
+  <si>
+    <t>zc4028</t>
+  </si>
+  <si>
+    <t>zc4047</t>
+  </si>
+  <si>
+    <t>zc4053</t>
+  </si>
+  <si>
+    <t>zc4070</t>
+  </si>
+  <si>
     <t>ZC4077</t>
   </si>
   <si>
+    <t>zc4510</t>
+  </si>
+  <si>
     <t>ZC4520</t>
   </si>
   <si>
-    <t>ZC1800</t>
+    <t>zc4800</t>
   </si>
   <si>
     <t>ZC4811</t>
@@ -1410,6 +1488,765 @@
   </si>
   <si>
     <t>ZC4835</t>
+  </si>
+  <si>
+    <t>zt2289</t>
+  </si>
+  <si>
+    <t>zt2294</t>
+  </si>
+  <si>
+    <t>zt2320</t>
+  </si>
+  <si>
+    <t>zt2452</t>
+  </si>
+  <si>
+    <t>zt2467</t>
+  </si>
+  <si>
+    <t>zv1508</t>
+  </si>
+  <si>
+    <t>zv1525</t>
+  </si>
+  <si>
+    <t>zv1542</t>
+  </si>
+  <si>
+    <t>zv1610</t>
+  </si>
+  <si>
+    <t>zv1635</t>
+  </si>
+  <si>
+    <t>zv1642</t>
+  </si>
+  <si>
+    <t>zv1654</t>
+  </si>
+  <si>
+    <t>IC'S</t>
+  </si>
+  <si>
+    <t>zc4012</t>
+  </si>
+  <si>
+    <t>zc4018</t>
+  </si>
+  <si>
+    <t>zc4024</t>
+  </si>
+  <si>
+    <t>zc4029</t>
+  </si>
+  <si>
+    <t>zc4049</t>
+  </si>
+  <si>
+    <t>zc4056</t>
+  </si>
+  <si>
+    <t>zc4071</t>
+  </si>
+  <si>
+    <t>zc4081</t>
+  </si>
+  <si>
+    <t>zc4511</t>
+  </si>
+  <si>
+    <t>zc4528</t>
+  </si>
+  <si>
+    <t>zc4802</t>
+  </si>
+  <si>
+    <t>zc4821</t>
+  </si>
+  <si>
+    <t>zc4829</t>
+  </si>
+  <si>
+    <t>zc4837</t>
+  </si>
+  <si>
+    <t>zt2290</t>
+  </si>
+  <si>
+    <t>zt2297</t>
+  </si>
+  <si>
+    <t>zt2460</t>
+  </si>
+  <si>
+    <t>zt2468</t>
+  </si>
+  <si>
+    <t>zv1509</t>
+  </si>
+  <si>
+    <t>zv1530</t>
+  </si>
+  <si>
+    <t>zv1560</t>
+  </si>
+  <si>
+    <t>zv1615</t>
+  </si>
+  <si>
+    <t>zv1636</t>
+  </si>
+  <si>
+    <t>zv1644</t>
+  </si>
+  <si>
+    <t>zv1652</t>
+  </si>
+  <si>
+    <t>zc4001</t>
+  </si>
+  <si>
+    <t>zc4013</t>
+  </si>
+  <si>
+    <t>zc4022</t>
+  </si>
+  <si>
+    <t>zc4025</t>
+  </si>
+  <si>
+    <t>zc4030</t>
+  </si>
+  <si>
+    <t>zc4050</t>
+  </si>
+  <si>
+    <t>zc4060</t>
+  </si>
+  <si>
+    <t>zc4073</t>
+  </si>
+  <si>
+    <t>zc4093</t>
+  </si>
+  <si>
+    <t>zc4514</t>
+  </si>
+  <si>
+    <t>zc4538</t>
+  </si>
+  <si>
+    <t>zc4804</t>
+  </si>
+  <si>
+    <t>zc4823</t>
+  </si>
+  <si>
+    <t>zc4830</t>
+  </si>
+  <si>
+    <t>zc4838</t>
+  </si>
+  <si>
+    <t>zc4842</t>
+  </si>
+  <si>
+    <t>zc4850</t>
+  </si>
+  <si>
+    <t>zc4858</t>
+  </si>
+  <si>
+    <t>zc4869</t>
+  </si>
+  <si>
+    <t>zc4880</t>
+  </si>
+  <si>
+    <t>zk8821</t>
+  </si>
+  <si>
+    <t>zk8831</t>
+  </si>
+  <si>
+    <t>zk8864</t>
+  </si>
+  <si>
+    <t>zk8874</t>
+  </si>
+  <si>
+    <t>zl3071</t>
+  </si>
+  <si>
+    <t>zl3301</t>
+  </si>
+  <si>
+    <t>zl3334</t>
+  </si>
+  <si>
+    <t>zl3380</t>
+  </si>
+  <si>
+    <t>zl3455</t>
+  </si>
+  <si>
+    <t>zl3567</t>
+  </si>
+  <si>
+    <t>zl3752</t>
+  </si>
+  <si>
+    <t>zl3860</t>
+  </si>
+  <si>
+    <t>zl3936</t>
+  </si>
+  <si>
+    <t>zl3974</t>
+  </si>
+  <si>
+    <t>zs5002</t>
+  </si>
+  <si>
+    <t>zs5011</t>
+  </si>
+  <si>
+    <t>zs5032</t>
+  </si>
+  <si>
+    <t>zs5074</t>
+  </si>
+  <si>
+    <t>zs5090</t>
+  </si>
+  <si>
+    <t>zs5138</t>
+  </si>
+  <si>
+    <t>zs5157</t>
+  </si>
+  <si>
+    <t>zs5192</t>
+  </si>
+  <si>
+    <t>zs5244</t>
+  </si>
+  <si>
+    <t>zc4844</t>
+  </si>
+  <si>
+    <t>zc4853</t>
+  </si>
+  <si>
+    <t>zc4862</t>
+  </si>
+  <si>
+    <t>zc4870</t>
+  </si>
+  <si>
+    <t>zc4890</t>
+  </si>
+  <si>
+    <t>zk8824</t>
+  </si>
+  <si>
+    <t>zk8837</t>
+  </si>
+  <si>
+    <t>zk8866</t>
+  </si>
+  <si>
+    <t>zk8879</t>
+  </si>
+  <si>
+    <t>zl3072</t>
+  </si>
+  <si>
+    <t>zl3308</t>
+  </si>
+  <si>
+    <t>zl3336</t>
+  </si>
+  <si>
+    <t>zl3386</t>
+  </si>
+  <si>
+    <t>zl3482</t>
+  </si>
+  <si>
+    <t>zl3600</t>
+  </si>
+  <si>
+    <t>zl3753</t>
+  </si>
+  <si>
+    <t>zl3900</t>
+  </si>
+  <si>
+    <t>zl3956</t>
+  </si>
+  <si>
+    <t>zl3976</t>
+  </si>
+  <si>
+    <t>zs5004</t>
+  </si>
+  <si>
+    <t>zs5014</t>
+  </si>
+  <si>
+    <t>zs5042</t>
+  </si>
+  <si>
+    <t>zs5075</t>
+  </si>
+  <si>
+    <t>zs5093</t>
+  </si>
+  <si>
+    <t>zs5139</t>
+  </si>
+  <si>
+    <t>zs5161</t>
+  </si>
+  <si>
+    <t>zs5193</t>
+  </si>
+  <si>
+    <t>zs5245</t>
+  </si>
+  <si>
+    <t>zc4846</t>
+  </si>
+  <si>
+    <t>zc4855</t>
+  </si>
+  <si>
+    <t>zc4864</t>
+  </si>
+  <si>
+    <t>zc4872</t>
+  </si>
+  <si>
+    <t>zc4892</t>
+  </si>
+  <si>
+    <t>zk8825</t>
+  </si>
+  <si>
+    <t>zk8850</t>
+  </si>
+  <si>
+    <t>zk8868</t>
+  </si>
+  <si>
+    <t>zk8880</t>
+  </si>
+  <si>
+    <t>zl3074</t>
+  </si>
+  <si>
+    <t>zl3311</t>
+  </si>
+  <si>
+    <t>zl3348</t>
+  </si>
+  <si>
+    <t>zl3388</t>
+  </si>
+  <si>
+    <t>zl3484</t>
+  </si>
+  <si>
+    <t>zl3755</t>
+  </si>
+  <si>
+    <t>zl3914</t>
+  </si>
+  <si>
+    <t>zl3970</t>
+  </si>
+  <si>
+    <t>zl3995</t>
+  </si>
+  <si>
+    <t>zs5005</t>
+  </si>
+  <si>
+    <t>zs5020</t>
+  </si>
+  <si>
+    <t>zs5047</t>
+  </si>
+  <si>
+    <t>zs5076</t>
+  </si>
+  <si>
+    <t>zs5109</t>
+  </si>
+  <si>
+    <t>zs5151</t>
+  </si>
+  <si>
+    <t>zs5164</t>
+  </si>
+  <si>
+    <t>zs5221</t>
+  </si>
+  <si>
+    <t>zs5263</t>
+  </si>
+  <si>
+    <t>zc4848</t>
+  </si>
+  <si>
+    <t>zc4856</t>
+  </si>
+  <si>
+    <t>zc4865</t>
+  </si>
+  <si>
+    <t>zc4874</t>
+  </si>
+  <si>
+    <t>zc4895</t>
+  </si>
+  <si>
+    <t>zk8829</t>
+  </si>
+  <si>
+    <t>zk8855</t>
+  </si>
+  <si>
+    <t>zk8869</t>
+  </si>
+  <si>
+    <t>zk8882</t>
+  </si>
+  <si>
+    <t>zl3078</t>
+  </si>
+  <si>
+    <t>zl3319</t>
+  </si>
+  <si>
+    <t>zl3339</t>
+  </si>
+  <si>
+    <t>zl3393</t>
+  </si>
+  <si>
+    <t>zl3555</t>
+  </si>
+  <si>
+    <t>zl3741</t>
+  </si>
+  <si>
+    <t>zl3833</t>
+  </si>
+  <si>
+    <t>zl3915</t>
+  </si>
+  <si>
+    <t>zl3971</t>
+  </si>
+  <si>
+    <t>zs5000</t>
+  </si>
+  <si>
+    <t>zs5008</t>
+  </si>
+  <si>
+    <t>zs5027</t>
+  </si>
+  <si>
+    <t>zs5048</t>
+  </si>
+  <si>
+    <t>zs5085</t>
+  </si>
+  <si>
+    <t>zs5123</t>
+  </si>
+  <si>
+    <t>zs5153</t>
+  </si>
+  <si>
+    <t>zs5174</t>
+  </si>
+  <si>
+    <t>zs5240</t>
+  </si>
+  <si>
+    <t>zs5273</t>
+  </si>
+  <si>
+    <t>zc4849</t>
+  </si>
+  <si>
+    <t>zc4857</t>
+  </si>
+  <si>
+    <t>zc4867</t>
+  </si>
+  <si>
+    <t>zc4875</t>
+  </si>
+  <si>
+    <t>zc4914</t>
+  </si>
+  <si>
+    <t>zk8830</t>
+  </si>
+  <si>
+    <t>zk8862</t>
+  </si>
+  <si>
+    <t>zk8884</t>
+  </si>
+  <si>
+    <t>zl3084</t>
+  </si>
+  <si>
+    <t>zl3324</t>
+  </si>
+  <si>
+    <t>zl3358</t>
+  </si>
+  <si>
+    <t>zl3405</t>
+  </si>
+  <si>
+    <t>zl3556</t>
+  </si>
+  <si>
+    <t>zl3747</t>
+  </si>
+  <si>
+    <t>zl3835</t>
+  </si>
+  <si>
+    <t>zl3930</t>
+  </si>
+  <si>
+    <t>zl3972</t>
+  </si>
+  <si>
+    <t>zs5001</t>
+  </si>
+  <si>
+    <t>zs5010</t>
+  </si>
+  <si>
+    <t>zs5030</t>
+  </si>
+  <si>
+    <t>zs5073</t>
+  </si>
+  <si>
+    <t>zs5086</t>
+  </si>
+  <si>
+    <t>zs5125</t>
+  </si>
+  <si>
+    <t>zs5155</t>
+  </si>
+  <si>
+    <t>zs5175</t>
+  </si>
+  <si>
+    <t>zs5241</t>
+  </si>
+  <si>
+    <t>zs5274</t>
+  </si>
+  <si>
+    <t>zs5373</t>
+  </si>
+  <si>
+    <t>zx7010</t>
+  </si>
+  <si>
+    <t>zx7149</t>
+  </si>
+  <si>
+    <t>zz8202</t>
+  </si>
+  <si>
+    <t>zz8520</t>
+  </si>
+  <si>
+    <t>zz8570</t>
+  </si>
+  <si>
+    <t>zz8605</t>
+  </si>
+  <si>
+    <t>zz8770</t>
+  </si>
+  <si>
+    <t>zz8952</t>
+  </si>
+  <si>
+    <t>DC Plugs &amp; Skts</t>
+  </si>
+  <si>
+    <t>ps0518</t>
+  </si>
+  <si>
+    <t>pa3701</t>
+  </si>
+  <si>
+    <t>pa3692</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>pa0618</t>
+  </si>
+  <si>
+    <t>pa0626</t>
+  </si>
+  <si>
+    <t>pa0631</t>
+  </si>
+  <si>
+    <t>pp0590</t>
+  </si>
+  <si>
+    <t>MOV</t>
+  </si>
+  <si>
+    <t>rn3412</t>
+  </si>
+  <si>
+    <t>rn3438</t>
+  </si>
+  <si>
+    <t>zs5804</t>
+  </si>
+  <si>
+    <t>zx7012</t>
+  </si>
+  <si>
+    <t>zx7192</t>
+  </si>
+  <si>
+    <t>zz8480</t>
+  </si>
+  <si>
+    <t>zz8530</t>
+  </si>
+  <si>
+    <t>zz8575</t>
+  </si>
+  <si>
+    <t>pa0611</t>
+  </si>
+  <si>
+    <t>pa0620</t>
+  </si>
+  <si>
+    <t>pa0632</t>
+  </si>
+  <si>
+    <t>pp0631</t>
+  </si>
+  <si>
+    <t>ps0592</t>
+  </si>
+  <si>
+    <t>rn3400</t>
+  </si>
+  <si>
+    <t>rn3413</t>
+  </si>
+  <si>
+    <t>rn3440</t>
+  </si>
+  <si>
+    <t>zs5806</t>
+  </si>
+  <si>
+    <t>zx7141</t>
+  </si>
+  <si>
+    <t>zz8148</t>
+  </si>
+  <si>
+    <t>zz8485</t>
+  </si>
+  <si>
+    <t>zz8540</t>
+  </si>
+  <si>
+    <t>zz8600</t>
+  </si>
+  <si>
+    <t>pa0612</t>
+  </si>
+  <si>
+    <t>pa0621</t>
+  </si>
+  <si>
+    <t>zs5807</t>
+  </si>
+  <si>
+    <t>zx7145</t>
+  </si>
+  <si>
+    <t>zz8149</t>
+  </si>
+  <si>
+    <t>zz8471</t>
+  </si>
+  <si>
+    <t>zz8550</t>
+  </si>
+  <si>
+    <t>zz8602</t>
+  </si>
+  <si>
+    <t>zx7006</t>
+  </si>
+  <si>
+    <t>zx7147</t>
+  </si>
+  <si>
+    <t>zz8200</t>
+  </si>
+  <si>
+    <t>zz8500</t>
+  </si>
+  <si>
+    <t>zz8560</t>
+  </si>
+  <si>
+    <t>POLYSWITCH</t>
+  </si>
+  <si>
+    <t>rn3468</t>
+  </si>
+  <si>
+    <t>rq5272</t>
+  </si>
+  <si>
+    <t>rq5278</t>
+  </si>
+  <si>
+    <t>rq5289</t>
+  </si>
+  <si>
+    <t>rq5299</t>
+  </si>
+  <si>
+    <t>IC Sockets</t>
+  </si>
+  <si>
+    <t>rn3460</t>
   </si>
 </sst>
 </file>
@@ -1417,12 +2254,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1454,29 +2291,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1490,14 +2312,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1506,16 +2320,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1529,6 +2343,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -1537,10 +2358,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1561,7 +2391,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1569,14 +2399,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1609,7 +2439,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1621,37 +2463,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1663,31 +2493,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1705,7 +2517,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1717,61 +2595,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1803,8 +2633,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1820,24 +2659,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1882,94 +2703,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1978,64 +2808,68 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="29"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="10"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2355,15 +3189,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AC44"/>
+  <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
+    <col min="2" max="2" width="13.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="11.2857142857143" customWidth="1"/>
     <col min="7" max="7" width="7.85714285714286" customWidth="1"/>
     <col min="8" max="9" width="12.1428571428571" customWidth="1"/>
@@ -2886,12 +3720,14 @@
       <c r="U6" t="s">
         <v>129</v>
       </c>
+      <c r="V6" s="5"/>
       <c r="W6" t="s">
         <v>130</v>
       </c>
       <c r="X6" t="s">
         <v>131</v>
       </c>
+      <c r="Y6" s="5"/>
       <c r="Z6" t="s">
         <v>132</v>
       </c>
@@ -2936,10 +3772,11 @@
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
     </row>
-    <row r="8" ht="15.75" spans="1:29">
+    <row r="8" spans="1:29">
       <c r="A8" s="2">
         <v>6</v>
       </c>
+      <c r="B8" s="5"/>
       <c r="C8" t="s">
         <v>136</v>
       </c>
@@ -3338,12 +4175,16 @@
       <c r="P12" t="s">
         <v>260</v>
       </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
       <c r="S12" t="s">
         <v>261</v>
       </c>
+      <c r="T12" s="5"/>
       <c r="U12" t="s">
         <v>262</v>
       </c>
+      <c r="V12" s="5"/>
       <c r="W12" t="s">
         <v>263</v>
       </c>
@@ -3873,7 +4714,7 @@
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
     </row>
-    <row r="20" ht="15.75" spans="1:29">
+    <row r="20" spans="1:29">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -3889,6 +4730,7 @@
       <c r="E20" t="s">
         <v>411</v>
       </c>
+      <c r="F20" s="5"/>
       <c r="G20" t="s">
         <v>412</v>
       </c>
@@ -3981,191 +4823,1159 @@
       <c r="G21" t="s">
         <v>440</v>
       </c>
+      <c r="H21" t="s">
+        <v>441</v>
+      </c>
+      <c r="I21" t="s">
+        <v>442</v>
+      </c>
+      <c r="J21" t="s">
+        <v>443</v>
+      </c>
       <c r="K21" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="L21" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="M21" t="s">
-        <v>443</v>
+        <v>446</v>
+      </c>
+      <c r="N21" t="s">
+        <v>447</v>
       </c>
       <c r="O21" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="P21" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="Q21" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="R21" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="S21" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="T21" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="U21" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="V21" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="W21" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="X21" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="Y21" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="Z21" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="AA21" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="AB21" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="AC21" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="2">
         <v>18</v>
       </c>
+      <c r="B22" t="s">
+        <v>463</v>
+      </c>
+      <c r="C22" t="s">
+        <v>464</v>
+      </c>
+      <c r="D22" t="s">
+        <v>465</v>
+      </c>
+      <c r="E22" t="s">
+        <v>466</v>
+      </c>
+      <c r="F22" t="s">
+        <v>467</v>
+      </c>
+      <c r="G22" t="s">
+        <v>468</v>
+      </c>
+      <c r="H22" t="s">
+        <v>469</v>
+      </c>
+      <c r="I22" t="s">
+        <v>470</v>
+      </c>
+      <c r="J22" t="s">
+        <v>471</v>
+      </c>
+      <c r="K22" t="s">
+        <v>472</v>
+      </c>
+      <c r="L22" t="s">
+        <v>473</v>
+      </c>
+      <c r="M22" t="s">
+        <v>474</v>
+      </c>
+      <c r="N22" t="s">
+        <v>475</v>
+      </c>
+      <c r="O22" t="s">
+        <v>476</v>
+      </c>
+      <c r="P22" t="s">
+        <v>477</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>478</v>
+      </c>
+      <c r="R22" t="s">
+        <v>479</v>
+      </c>
+      <c r="S22" t="s">
+        <v>480</v>
+      </c>
+      <c r="T22" t="s">
+        <v>481</v>
+      </c>
+      <c r="U22" t="s">
+        <v>482</v>
+      </c>
+      <c r="V22" t="s">
+        <v>483</v>
+      </c>
       <c r="W22" t="s">
-        <v>459</v>
+        <v>484</v>
+      </c>
+      <c r="X22" t="s">
+        <v>485</v>
       </c>
       <c r="Y22" t="s">
-        <v>460</v>
+        <v>486</v>
       </c>
       <c r="Z22" t="s">
-        <v>461</v>
+        <v>487</v>
       </c>
       <c r="AA22" t="s">
-        <v>462</v>
+        <v>488</v>
       </c>
       <c r="AB22" t="s">
-        <v>463</v>
+        <v>489</v>
       </c>
       <c r="AC22" t="s">
-        <v>464</v>
+        <v>490</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:29">
       <c r="A23" s="2">
         <v>19</v>
       </c>
+      <c r="B23" t="s">
+        <v>491</v>
+      </c>
+      <c r="C23" t="s">
+        <v>492</v>
+      </c>
+      <c r="D23" t="s">
+        <v>493</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" t="s">
+        <v>494</v>
+      </c>
+      <c r="G23" t="s">
+        <v>495</v>
+      </c>
+      <c r="H23" t="s">
+        <v>496</v>
+      </c>
+      <c r="I23" t="s">
+        <v>497</v>
+      </c>
+      <c r="J23" t="s">
+        <v>498</v>
+      </c>
+      <c r="K23" t="s">
+        <v>499</v>
+      </c>
+      <c r="L23" t="s">
+        <v>500</v>
+      </c>
+      <c r="M23" t="s">
+        <v>501</v>
+      </c>
+      <c r="N23" t="s">
+        <v>502</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="P23" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>505</v>
+      </c>
+      <c r="R23" t="s">
+        <v>506</v>
+      </c>
+      <c r="S23" t="s">
+        <v>507</v>
+      </c>
+      <c r="T23" t="s">
+        <v>508</v>
+      </c>
+      <c r="U23" t="s">
+        <v>509</v>
+      </c>
+      <c r="V23" t="s">
+        <v>510</v>
+      </c>
+      <c r="W23" t="s">
+        <v>511</v>
+      </c>
+      <c r="X23" t="s">
+        <v>512</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>513</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>514</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>515</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>516</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>517</v>
+      </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" ht="15.75" spans="1:29">
       <c r="A24" s="2">
         <v>20</v>
       </c>
+      <c r="B24" t="s">
+        <v>518</v>
+      </c>
+      <c r="C24" t="s">
+        <v>519</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" t="s">
+        <v>520</v>
+      </c>
+      <c r="G24" t="s">
+        <v>521</v>
+      </c>
+      <c r="H24" t="s">
+        <v>522</v>
+      </c>
+      <c r="I24" t="s">
+        <v>523</v>
+      </c>
+      <c r="J24" t="s">
+        <v>524</v>
+      </c>
+      <c r="K24" t="s">
+        <v>525</v>
+      </c>
+      <c r="L24" t="s">
+        <v>526</v>
+      </c>
+      <c r="M24" t="s">
+        <v>527</v>
+      </c>
+      <c r="N24" t="s">
+        <v>528</v>
+      </c>
+      <c r="O24" t="s">
+        <v>529</v>
+      </c>
+      <c r="P24" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>531</v>
+      </c>
+      <c r="R24" t="s">
+        <v>532</v>
+      </c>
+      <c r="S24" t="s">
+        <v>533</v>
+      </c>
+      <c r="T24" t="s">
+        <v>534</v>
+      </c>
+      <c r="U24" t="s">
+        <v>535</v>
+      </c>
+      <c r="V24" t="s">
+        <v>536</v>
+      </c>
+      <c r="W24" t="s">
+        <v>537</v>
+      </c>
+      <c r="X24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>539</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>540</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>541</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>542</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="2">
+    <row r="25" ht="4" customHeight="1" spans="1:29">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+    </row>
+    <row r="26" ht="15.75" spans="1:29">
+      <c r="A26" s="2">
         <v>21</v>
       </c>
+      <c r="B26" t="s">
+        <v>544</v>
+      </c>
+      <c r="C26" t="s">
+        <v>545</v>
+      </c>
+      <c r="D26" t="s">
+        <v>546</v>
+      </c>
+      <c r="E26" t="s">
+        <v>547</v>
+      </c>
+      <c r="F26" t="s">
+        <v>548</v>
+      </c>
+      <c r="G26" t="s">
+        <v>549</v>
+      </c>
+      <c r="H26" t="s">
+        <v>550</v>
+      </c>
+      <c r="I26" t="s">
+        <v>551</v>
+      </c>
+      <c r="J26" t="s">
+        <v>552</v>
+      </c>
+      <c r="K26" t="s">
+        <v>553</v>
+      </c>
+      <c r="L26" t="s">
+        <v>554</v>
+      </c>
+      <c r="M26" t="s">
+        <v>555</v>
+      </c>
+      <c r="N26" t="s">
+        <v>556</v>
+      </c>
+      <c r="O26" t="s">
+        <v>557</v>
+      </c>
+      <c r="P26" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>559</v>
+      </c>
+      <c r="R26" t="s">
+        <v>560</v>
+      </c>
+      <c r="S26" t="s">
+        <v>561</v>
+      </c>
+      <c r="T26" t="s">
+        <v>562</v>
+      </c>
+      <c r="U26" t="s">
+        <v>563</v>
+      </c>
+      <c r="V26" t="s">
+        <v>564</v>
+      </c>
+      <c r="W26" t="s">
+        <v>565</v>
+      </c>
+      <c r="X26" t="s">
+        <v>566</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>567</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>568</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>569</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>570</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="2">
+    <row r="27" spans="1:29">
+      <c r="A27" s="2">
         <v>22</v>
       </c>
+      <c r="B27" t="s">
+        <v>572</v>
+      </c>
+      <c r="C27" t="s">
+        <v>573</v>
+      </c>
+      <c r="D27" t="s">
+        <v>574</v>
+      </c>
+      <c r="E27" t="s">
+        <v>575</v>
+      </c>
+      <c r="F27" t="s">
+        <v>576</v>
+      </c>
+      <c r="G27" t="s">
+        <v>577</v>
+      </c>
+      <c r="H27" t="s">
+        <v>578</v>
+      </c>
+      <c r="I27" t="s">
+        <v>579</v>
+      </c>
+      <c r="J27" t="s">
+        <v>580</v>
+      </c>
+      <c r="K27" t="s">
+        <v>581</v>
+      </c>
+      <c r="L27" t="s">
+        <v>582</v>
+      </c>
+      <c r="M27" t="s">
+        <v>583</v>
+      </c>
+      <c r="N27" t="s">
+        <v>584</v>
+      </c>
+      <c r="O27" t="s">
+        <v>585</v>
+      </c>
+      <c r="P27" t="s">
+        <v>586</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>587</v>
+      </c>
+      <c r="R27" t="s">
+        <v>588</v>
+      </c>
+      <c r="S27" t="s">
+        <v>589</v>
+      </c>
+      <c r="T27" t="s">
+        <v>590</v>
+      </c>
+      <c r="U27" t="s">
+        <v>591</v>
+      </c>
+      <c r="V27" t="s">
+        <v>592</v>
+      </c>
+      <c r="W27" t="s">
+        <v>593</v>
+      </c>
+      <c r="X27" t="s">
+        <v>594</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>595</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>596</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>597</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>598</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="2">
+    <row r="28" spans="1:29">
+      <c r="A28" s="2">
         <v>23</v>
       </c>
+      <c r="B28" t="s">
+        <v>600</v>
+      </c>
+      <c r="C28" t="s">
+        <v>601</v>
+      </c>
+      <c r="D28" t="s">
+        <v>602</v>
+      </c>
+      <c r="E28" t="s">
+        <v>603</v>
+      </c>
+      <c r="F28" t="s">
+        <v>604</v>
+      </c>
+      <c r="G28" t="s">
+        <v>605</v>
+      </c>
+      <c r="H28" t="s">
+        <v>606</v>
+      </c>
+      <c r="I28" t="s">
+        <v>607</v>
+      </c>
+      <c r="J28" t="s">
+        <v>608</v>
+      </c>
+      <c r="K28" t="s">
+        <v>609</v>
+      </c>
+      <c r="L28" t="s">
+        <v>610</v>
+      </c>
+      <c r="M28" t="s">
+        <v>611</v>
+      </c>
+      <c r="N28" t="s">
+        <v>612</v>
+      </c>
+      <c r="O28" t="s">
+        <v>613</v>
+      </c>
+      <c r="P28" s="5"/>
+      <c r="Q28" t="s">
+        <v>614</v>
+      </c>
+      <c r="R28" t="s">
+        <v>615</v>
+      </c>
+      <c r="S28" t="s">
+        <v>616</v>
+      </c>
+      <c r="T28" t="s">
+        <v>617</v>
+      </c>
+      <c r="U28" t="s">
+        <v>618</v>
+      </c>
+      <c r="V28" t="s">
+        <v>619</v>
+      </c>
+      <c r="W28" t="s">
+        <v>620</v>
+      </c>
+      <c r="X28" t="s">
+        <v>621</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>622</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>623</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>624</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>625</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>626</v>
+      </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="2">
+    <row r="29" spans="1:29">
+      <c r="A29" s="2">
         <v>24</v>
       </c>
+      <c r="B29" t="s">
+        <v>627</v>
+      </c>
+      <c r="C29" t="s">
+        <v>628</v>
+      </c>
+      <c r="D29" t="s">
+        <v>629</v>
+      </c>
+      <c r="E29" t="s">
+        <v>630</v>
+      </c>
+      <c r="F29" t="s">
+        <v>631</v>
+      </c>
+      <c r="G29" t="s">
+        <v>632</v>
+      </c>
+      <c r="H29" t="s">
+        <v>633</v>
+      </c>
+      <c r="I29" t="s">
+        <v>634</v>
+      </c>
+      <c r="J29" t="s">
+        <v>635</v>
+      </c>
+      <c r="K29" t="s">
+        <v>636</v>
+      </c>
+      <c r="L29" t="s">
+        <v>637</v>
+      </c>
+      <c r="M29" t="s">
+        <v>638</v>
+      </c>
+      <c r="N29" t="s">
+        <v>639</v>
+      </c>
+      <c r="O29" t="s">
+        <v>640</v>
+      </c>
+      <c r="P29" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>642</v>
+      </c>
+      <c r="R29" t="s">
+        <v>643</v>
+      </c>
+      <c r="S29" t="s">
+        <v>644</v>
+      </c>
+      <c r="T29" t="s">
+        <v>645</v>
+      </c>
+      <c r="U29" t="s">
+        <v>646</v>
+      </c>
+      <c r="V29" t="s">
+        <v>647</v>
+      </c>
+      <c r="W29" t="s">
+        <v>648</v>
+      </c>
+      <c r="X29" t="s">
+        <v>649</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>650</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>651</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>652</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>653</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>654</v>
+      </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="2">
+    <row r="30" ht="15.75" spans="1:29">
+      <c r="A30" s="2">
         <v>25</v>
       </c>
+      <c r="B30" t="s">
+        <v>655</v>
+      </c>
+      <c r="C30" t="s">
+        <v>656</v>
+      </c>
+      <c r="D30" t="s">
+        <v>657</v>
+      </c>
+      <c r="E30" t="s">
+        <v>658</v>
+      </c>
+      <c r="F30" t="s">
+        <v>659</v>
+      </c>
+      <c r="G30" t="s">
+        <v>660</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="I30" s="5"/>
+      <c r="J30" t="s">
+        <v>662</v>
+      </c>
+      <c r="K30" t="s">
+        <v>663</v>
+      </c>
+      <c r="L30" t="s">
+        <v>664</v>
+      </c>
+      <c r="M30" t="s">
+        <v>665</v>
+      </c>
+      <c r="N30" t="s">
+        <v>666</v>
+      </c>
+      <c r="O30" t="s">
+        <v>667</v>
+      </c>
+      <c r="P30" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>669</v>
+      </c>
+      <c r="R30" t="s">
+        <v>670</v>
+      </c>
+      <c r="S30" t="s">
+        <v>671</v>
+      </c>
+      <c r="T30" t="s">
+        <v>672</v>
+      </c>
+      <c r="U30" t="s">
+        <v>673</v>
+      </c>
+      <c r="V30" t="s">
+        <v>674</v>
+      </c>
+      <c r="W30" t="s">
+        <v>675</v>
+      </c>
+      <c r="X30" t="s">
+        <v>676</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>677</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>680</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>681</v>
+      </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="2">
+    <row r="31" ht="4" customHeight="1" spans="1:29">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+    </row>
+    <row r="32" ht="15.75" spans="1:29">
+      <c r="A32" s="2">
         <v>26</v>
       </c>
+      <c r="B32" t="s">
+        <v>682</v>
+      </c>
+      <c r="C32" t="s">
+        <v>683</v>
+      </c>
+      <c r="D32" t="s">
+        <v>684</v>
+      </c>
+      <c r="E32" t="s">
+        <v>685</v>
+      </c>
+      <c r="F32" t="s">
+        <v>686</v>
+      </c>
+      <c r="G32" t="s">
+        <v>687</v>
+      </c>
+      <c r="H32" t="s">
+        <v>688</v>
+      </c>
+      <c r="J32" t="s">
+        <v>689</v>
+      </c>
+      <c r="K32" t="s">
+        <v>690</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="O32" t="s">
+        <v>692</v>
+      </c>
+      <c r="R32" t="s">
+        <v>693</v>
+      </c>
+      <c r="S32" t="s">
+        <v>694</v>
+      </c>
+      <c r="T32" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="U32" t="s">
+        <v>696</v>
+      </c>
+      <c r="V32" t="s">
+        <v>697</v>
+      </c>
+      <c r="W32" t="s">
+        <v>698</v>
+      </c>
+      <c r="X32" s="5"/>
+      <c r="Y32" t="s">
+        <v>699</v>
+      </c>
+      <c r="Z32" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>701</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>702</v>
+      </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="2">
+    <row r="33" spans="1:29">
+      <c r="A33" s="2">
         <v>27</v>
       </c>
+      <c r="B33" t="s">
+        <v>703</v>
+      </c>
+      <c r="C33" t="s">
+        <v>704</v>
+      </c>
+      <c r="D33" t="s">
+        <v>705</v>
+      </c>
+      <c r="E33" t="s">
+        <v>706</v>
+      </c>
+      <c r="F33" t="s">
+        <v>707</v>
+      </c>
+      <c r="G33" t="s">
+        <v>708</v>
+      </c>
+      <c r="T33" t="s">
+        <v>709</v>
+      </c>
+      <c r="U33" t="s">
+        <v>710</v>
+      </c>
+      <c r="W33" t="s">
+        <v>711</v>
+      </c>
+      <c r="X33" t="s">
+        <v>712</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>713</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>714</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>715</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>716</v>
+      </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="2">
+    <row r="34" spans="1:21">
+      <c r="A34" s="2">
         <v>28</v>
       </c>
+      <c r="B34" t="s">
+        <v>717</v>
+      </c>
+      <c r="C34" t="s">
+        <v>718</v>
+      </c>
+      <c r="D34" t="s">
+        <v>719</v>
+      </c>
+      <c r="E34" t="s">
+        <v>720</v>
+      </c>
+      <c r="F34" t="s">
+        <v>721</v>
+      </c>
+      <c r="G34" t="s">
+        <v>722</v>
+      </c>
+      <c r="T34" t="s">
+        <v>723</v>
+      </c>
+      <c r="U34" t="s">
+        <v>724</v>
+      </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="2">
+    <row r="35" spans="1:7">
+      <c r="A35" s="2">
         <v>29</v>
       </c>
+      <c r="B35" t="s">
+        <v>725</v>
+      </c>
+      <c r="C35" t="s">
+        <v>726</v>
+      </c>
+      <c r="D35" t="s">
+        <v>727</v>
+      </c>
+      <c r="E35" t="s">
+        <v>728</v>
+      </c>
+      <c r="F35" t="s">
+        <v>729</v>
+      </c>
+      <c r="G35" t="s">
+        <v>730</v>
+      </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="2">
+    <row r="36" ht="15.75" spans="1:7">
+      <c r="A36" s="2">
         <v>30</v>
       </c>
+      <c r="B36" t="s">
+        <v>731</v>
+      </c>
+      <c r="C36" t="s">
+        <v>732</v>
+      </c>
+      <c r="D36" t="s">
+        <v>733</v>
+      </c>
+      <c r="E36" t="s">
+        <v>734</v>
+      </c>
+      <c r="F36" t="s">
+        <v>735</v>
+      </c>
+      <c r="G36" s="5"/>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="2">
+    <row r="37" ht="4" customHeight="1" spans="1:29">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="4"/>
+    </row>
+    <row r="38" ht="15.75" spans="1:8">
+      <c r="A38" s="2">
         <v>31</v>
       </c>
+      <c r="B38" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="C38" t="s">
+        <v>737</v>
+      </c>
+      <c r="D38" t="s">
+        <v>738</v>
+      </c>
+      <c r="E38" t="s">
+        <v>739</v>
+      </c>
+      <c r="F38" t="s">
+        <v>740</v>
+      </c>
+      <c r="G38" t="s">
+        <v>741</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>742</v>
+      </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2">
+    <row r="39" spans="1:2">
+      <c r="A39" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="2">
-        <v>35</v>
+      <c r="B39" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="2">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" spans="1:1">
+      <c r="A42" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" ht="4" customHeight="1" spans="1:29">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
+    </row>
+    <row r="44" ht="15.75" spans="1:1">
+      <c r="A44" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="2">
+    <row r="46" spans="1:1">
+      <c r="A46" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="2">
+    <row r="47" spans="1:1">
+      <c r="A47" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="2">
+    <row r="48" spans="1:1">
+      <c r="A48" s="2">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected Z tray Readout
</commit_message>
<xml_diff>
--- a/Active Projects/Work Z-tray Readout.xlsx
+++ b/Active Projects/Work Z-tray Readout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21210" windowHeight="8205"/>
+    <workbookView windowWidth="19890" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="747">
   <si>
     <t>LED'S</t>
   </si>
@@ -1499,6 +1499,9 @@
     <t>zt2320</t>
   </si>
   <si>
+    <t>zt2375</t>
+  </si>
+  <si>
     <t>zt2452</t>
   </si>
   <si>
@@ -1575,6 +1578,12 @@
   </si>
   <si>
     <t>zt2297</t>
+  </si>
+  <si>
+    <t>zt2322</t>
+  </si>
+  <si>
+    <t>zt2397</t>
   </si>
   <si>
     <t>zt2460</t>
@@ -2254,10 +2263,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -2297,13 +2306,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -2312,18 +2314,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2343,24 +2352,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2376,20 +2377,28 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2406,7 +2415,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2445,7 +2454,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2457,13 +2472,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2475,31 +2538,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2511,7 +2556,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2523,25 +2580,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2553,55 +2610,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2630,11 +2639,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2663,6 +2678,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2678,17 +2702,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2703,19 +2721,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2733,10 +2742,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2748,58 +2757,58 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2808,68 +2817,67 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="23"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="29"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="23" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3192,7 +3200,7 @@
   <dimension ref="A1:AC48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3772,7 +3780,7 @@
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" ht="15.75" spans="1:29">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -4714,7 +4722,7 @@
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" ht="15.75" spans="1:29">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -4992,78 +5000,80 @@
       <c r="D23" t="s">
         <v>493</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>494</v>
+      </c>
       <c r="F23" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="G23" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H23" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="I23" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="J23" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="K23" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="L23" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="M23" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="N23" t="s">
-        <v>502</v>
-      </c>
-      <c r="O23" s="8" t="s">
         <v>503</v>
       </c>
+      <c r="O23" s="7" t="s">
+        <v>504</v>
+      </c>
       <c r="P23" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="Q23" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="R23" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="S23" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="T23" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="U23" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="V23" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="W23" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="X23" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="Y23" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="Z23" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AA23" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AB23" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AC23" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="1:29">
@@ -5071,84 +5081,88 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C24" t="s">
-        <v>519</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+        <v>520</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>522</v>
+      </c>
       <c r="F24" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="G24" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="H24" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="I24" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="J24" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="K24" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="L24" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="M24" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="N24" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="O24" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="P24" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="Q24" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="R24" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="S24" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="T24" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="U24" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="V24" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="W24" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="X24" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="Y24" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="Z24" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="AA24" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="AB24" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="AC24" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="25" ht="4" customHeight="1" spans="1:29">
@@ -5187,88 +5201,88 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="C26" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="D26" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="E26" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="F26" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G26" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="H26" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="I26" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="J26" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="K26" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="L26" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="M26" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="N26" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="O26" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="P26" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="Q26" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="R26" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="S26" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="T26" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="U26" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="V26" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="W26" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="X26" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="Y26" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="Z26" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="AA26" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="AB26" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="AC26" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -5276,88 +5290,88 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="C27" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D27" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="E27" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="F27" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="G27" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="H27" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="I27" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="J27" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="K27" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="L27" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="M27" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="N27" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="O27" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="P27" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="Q27" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="R27" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="S27" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="T27" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="U27" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="V27" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="W27" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="X27" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="Y27" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="Z27" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="AA27" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="AB27" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="AC27" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -5365,86 +5379,86 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C28" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D28" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="E28" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="F28" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="G28" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="H28" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="I28" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="J28" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="K28" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="L28" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="M28" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="N28" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="O28" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="P28" s="5"/>
       <c r="Q28" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="R28" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="S28" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="T28" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="U28" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="V28" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="W28" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="X28" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="Y28" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="Z28" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="AA28" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="AB28" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="AC28" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -5452,88 +5466,88 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="C29" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="D29" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="E29" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="F29" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="G29" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="H29" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="I29" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="J29" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="K29" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="L29" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="M29" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="N29" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="O29" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="P29" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="Q29" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="R29" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="S29" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="T29" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="U29" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="V29" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="W29" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="X29" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="Y29" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="Z29" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="AA29" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="AB29" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="AC29" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="30" ht="15.75" spans="1:29">
@@ -5541,86 +5555,86 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="C30" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D30" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="E30" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="F30" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="G30" t="s">
-        <v>660</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>661</v>
+        <v>663</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>664</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="K30" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="L30" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="M30" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="N30" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="O30" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="P30" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="Q30" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="R30" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="S30" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="T30" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="U30" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="V30" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="W30" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="X30" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="Y30" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="Z30" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="AA30" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="AB30" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="AC30" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="31" ht="4" customHeight="1" spans="1:29">
@@ -5659,68 +5673,68 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="C32" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="D32" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="E32" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="F32" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="G32" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="H32" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="J32" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="K32" t="s">
-        <v>690</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>691</v>
+        <v>693</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>694</v>
       </c>
       <c r="O32" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="R32" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="S32" t="s">
-        <v>694</v>
-      </c>
-      <c r="T32" s="8" t="s">
-        <v>695</v>
+        <v>697</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>698</v>
       </c>
       <c r="U32" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="V32" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="W32" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="X32" s="5"/>
       <c r="Y32" t="s">
-        <v>699</v>
-      </c>
-      <c r="Z32" s="8" t="s">
-        <v>700</v>
+        <v>702</v>
+      </c>
+      <c r="Z32" s="7" t="s">
+        <v>703</v>
       </c>
       <c r="AA32" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="AC32" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="33" spans="1:29">
@@ -5728,46 +5742,46 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="C33" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="D33" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="E33" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="F33" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="G33" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="T33" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="U33" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="W33" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="X33" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="Y33" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="Z33" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="AA33" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="AC33" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -5775,28 +5789,28 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="C34" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="D34" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="E34" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="F34" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="G34" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="T34" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="U34" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5804,22 +5818,22 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="C35" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="D35" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="E35" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F35" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="G35" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="36" ht="15.75" spans="1:7">
@@ -5827,19 +5841,19 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="C36" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="D36" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="E36" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="F36" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="G36" s="5"/>
     </row>
@@ -5878,26 +5892,26 @@
       <c r="A38" s="2">
         <v>31</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>736</v>
+      <c r="B38" s="7" t="s">
+        <v>739</v>
       </c>
       <c r="C38" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="D38" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="E38" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="F38" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G38" t="s">
-        <v>741</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>742</v>
+        <v>744</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5905,7 +5919,7 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
     </row>
     <row r="40" spans="1:1">

</xml_diff>

<commit_message>
Completed Z Tray Readout
</commit_message>
<xml_diff>
--- a/Active Projects/Work Z-tray Readout.xlsx
+++ b/Active Projects/Work Z-tray Readout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665"/>
+    <workbookView windowWidth="21210" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="1002">
   <si>
     <t>LED'S</t>
   </si>
@@ -2093,6 +2093,9 @@
     <t>zz8605</t>
   </si>
   <si>
+    <t>zz8750</t>
+  </si>
+  <si>
     <t>zz8770</t>
   </si>
   <si>
@@ -2102,9 +2105,21 @@
     <t>DC Plugs &amp; Skts</t>
   </si>
   <si>
+    <t>pp0507</t>
+  </si>
+  <si>
+    <t>pp0512</t>
+  </si>
+  <si>
     <t>ps0518</t>
   </si>
   <si>
+    <t>ps0526</t>
+  </si>
+  <si>
+    <t>pp0532</t>
+  </si>
+  <si>
     <t>pa3701</t>
   </si>
   <si>
@@ -2132,6 +2147,9 @@
     <t>rn3412</t>
   </si>
   <si>
+    <t>THERMISTORS</t>
+  </si>
+  <si>
     <t>rn3438</t>
   </si>
   <si>
@@ -2153,12 +2171,51 @@
     <t>zz8575</t>
   </si>
   <si>
+    <t>zz8700</t>
+  </si>
+  <si>
+    <t>zz8753</t>
+  </si>
+  <si>
+    <t>zz8772</t>
+  </si>
+  <si>
+    <t>zz8953</t>
+  </si>
+  <si>
+    <t>pp0502</t>
+  </si>
+  <si>
+    <t>pp0508</t>
+  </si>
+  <si>
+    <t>pp0513</t>
+  </si>
+  <si>
+    <t>ps0519</t>
+  </si>
+  <si>
+    <t>ps0528</t>
+  </si>
+  <si>
+    <t>ps0534</t>
+  </si>
+  <si>
+    <t>pa3702</t>
+  </si>
+  <si>
+    <t>ps0789</t>
+  </si>
+  <si>
     <t>pa0611</t>
   </si>
   <si>
     <t>pa0620</t>
   </si>
   <si>
+    <t>pa0627</t>
+  </si>
+  <si>
     <t>pa0632</t>
   </si>
   <si>
@@ -2174,6 +2231,9 @@
     <t>rn3413</t>
   </si>
   <si>
+    <t>rn3430</t>
+  </si>
+  <si>
     <t>rn3440</t>
   </si>
   <si>
@@ -2195,12 +2255,69 @@
     <t>zz8600</t>
   </si>
   <si>
+    <t>zz8710</t>
+  </si>
+  <si>
+    <t>zz8755</t>
+  </si>
+  <si>
+    <t>zz8900</t>
+  </si>
+  <si>
+    <t>pp0504</t>
+  </si>
+  <si>
+    <t>pp0509</t>
+  </si>
+  <si>
+    <t>pp0514</t>
+  </si>
+  <si>
+    <t>ps0520</t>
+  </si>
+  <si>
+    <t>ps0531</t>
+  </si>
+  <si>
+    <t>ps0536</t>
+  </si>
+  <si>
+    <t>pa3704</t>
+  </si>
+  <si>
+    <t>pa3711</t>
+  </si>
+  <si>
     <t>pa0612</t>
   </si>
   <si>
     <t>pa0621</t>
   </si>
   <si>
+    <t>pa0628</t>
+  </si>
+  <si>
+    <t>pa0635</t>
+  </si>
+  <si>
+    <t>pp0632</t>
+  </si>
+  <si>
+    <t>LDR's</t>
+  </si>
+  <si>
+    <t>rn3404</t>
+  </si>
+  <si>
+    <t>rn3415</t>
+  </si>
+  <si>
+    <t>rn3432</t>
+  </si>
+  <si>
+    <t>rn3442</t>
+  </si>
+  <si>
     <t>zs5807</t>
   </si>
   <si>
@@ -2219,6 +2336,66 @@
     <t>zz8602</t>
   </si>
   <si>
+    <t>zz8721</t>
+  </si>
+  <si>
+    <t>zz8760</t>
+  </si>
+  <si>
+    <t>zz8800</t>
+  </si>
+  <si>
+    <t>pp0505</t>
+  </si>
+  <si>
+    <t>pp0510</t>
+  </si>
+  <si>
+    <t>pp0515</t>
+  </si>
+  <si>
+    <t>ps0522</t>
+  </si>
+  <si>
+    <t>pp0531</t>
+  </si>
+  <si>
+    <t>ps0540</t>
+  </si>
+  <si>
+    <t>pa3706</t>
+  </si>
+  <si>
+    <t>pa3713</t>
+  </si>
+  <si>
+    <t>pa0613</t>
+  </si>
+  <si>
+    <t>pa0622</t>
+  </si>
+  <si>
+    <t>pa0629</t>
+  </si>
+  <si>
+    <t>pp0633</t>
+  </si>
+  <si>
+    <t>rd3480</t>
+  </si>
+  <si>
+    <t>rn3406</t>
+  </si>
+  <si>
+    <t>rn3416</t>
+  </si>
+  <si>
+    <t>rn3434</t>
+  </si>
+  <si>
+    <t>rn3444</t>
+  </si>
+  <si>
     <t>zx7006</t>
   </si>
   <si>
@@ -2234,6 +2411,66 @@
     <t>zz8560</t>
   </si>
   <si>
+    <t>zz8742</t>
+  </si>
+  <si>
+    <t>zz8765</t>
+  </si>
+  <si>
+    <t>zz8950</t>
+  </si>
+  <si>
+    <t>pp0506</t>
+  </si>
+  <si>
+    <t>pp0511</t>
+  </si>
+  <si>
+    <t>ps0516</t>
+  </si>
+  <si>
+    <t>ps0524</t>
+  </si>
+  <si>
+    <t>ps0532</t>
+  </si>
+  <si>
+    <t>pa3700</t>
+  </si>
+  <si>
+    <t>pa3707</t>
+  </si>
+  <si>
+    <t>st3933</t>
+  </si>
+  <si>
+    <t>pa0615</t>
+  </si>
+  <si>
+    <t>pa0624</t>
+  </si>
+  <si>
+    <t>pa0630</t>
+  </si>
+  <si>
+    <t>ps0634</t>
+  </si>
+  <si>
+    <t>rd3485</t>
+  </si>
+  <si>
+    <t>rn3411</t>
+  </si>
+  <si>
+    <t>rn3417</t>
+  </si>
+  <si>
+    <t>rn3436</t>
+  </si>
+  <si>
+    <t>rn3446</t>
+  </si>
+  <si>
     <t>POLYSWITCH</t>
   </si>
   <si>
@@ -2255,7 +2492,535 @@
     <t>IC Sockets</t>
   </si>
   <si>
+    <t>pi6458</t>
+  </si>
+  <si>
+    <t>pi6470</t>
+  </si>
+  <si>
+    <t>pi6484</t>
+  </si>
+  <si>
+    <t>pi6503</t>
+  </si>
+  <si>
+    <t>pi6508</t>
+  </si>
+  <si>
+    <t>pi6604</t>
+  </si>
+  <si>
+    <t>pi6628</t>
+  </si>
+  <si>
+    <t>ts1118</t>
+  </si>
+  <si>
+    <t>ts1312</t>
+  </si>
+  <si>
+    <t>ts1321</t>
+  </si>
+  <si>
+    <t>ts1352</t>
+  </si>
+  <si>
+    <t>ts1432</t>
+  </si>
+  <si>
+    <t>ts1466</t>
+  </si>
+  <si>
+    <t>ts1546</t>
+  </si>
+  <si>
+    <t>ts1557</t>
+  </si>
+  <si>
+    <t>ts1577</t>
+  </si>
+  <si>
+    <t>ts1587</t>
+  </si>
+  <si>
+    <t>ts1643</t>
+  </si>
+  <si>
+    <t>th1863</t>
+  </si>
+  <si>
     <t>rn3460</t>
+  </si>
+  <si>
+    <t>rn3470</t>
+  </si>
+  <si>
+    <t>rq5274</t>
+  </si>
+  <si>
+    <t>rq5279</t>
+  </si>
+  <si>
+    <t>rq5293</t>
+  </si>
+  <si>
+    <t>rr3420</t>
+  </si>
+  <si>
+    <t>pi6450</t>
+  </si>
+  <si>
+    <t>pi6460</t>
+  </si>
+  <si>
+    <t>pi6472</t>
+  </si>
+  <si>
+    <t>pi6499</t>
+  </si>
+  <si>
+    <t>pi6504</t>
+  </si>
+  <si>
+    <t>pi6510</t>
+  </si>
+  <si>
+    <t>pi6606</t>
+  </si>
+  <si>
+    <t>ps2080</t>
+  </si>
+  <si>
+    <t>ts1116</t>
+  </si>
+  <si>
+    <t>ts1306</t>
+  </si>
+  <si>
+    <t>ts1313</t>
+  </si>
+  <si>
+    <t>ts1322</t>
+  </si>
+  <si>
+    <t>ts1391</t>
+  </si>
+  <si>
+    <t>ts1436</t>
+  </si>
+  <si>
+    <t>ts1476</t>
+  </si>
+  <si>
+    <t>ts1518</t>
+  </si>
+  <si>
+    <t>ts1547</t>
+  </si>
+  <si>
+    <t>ts1566</t>
+  </si>
+  <si>
+    <t>ts1588</t>
+  </si>
+  <si>
+    <t>ts1644</t>
+  </si>
+  <si>
+    <t>td2420</t>
+  </si>
+  <si>
+    <t>rn3462</t>
+  </si>
+  <si>
+    <t>CRYSTALS</t>
+  </si>
+  <si>
+    <t>rq5275</t>
+  </si>
+  <si>
+    <t>rq5284</t>
+  </si>
+  <si>
+    <t>rq5296</t>
+  </si>
+  <si>
+    <t>pi6452</t>
+  </si>
+  <si>
+    <t>pi6462</t>
+  </si>
+  <si>
+    <t>pi6473</t>
+  </si>
+  <si>
+    <t>pi6500</t>
+  </si>
+  <si>
+    <t>pi6505</t>
+  </si>
+  <si>
+    <t>pi6550</t>
+  </si>
+  <si>
+    <t>pi6620</t>
+  </si>
+  <si>
+    <t>ps2082</t>
+  </si>
+  <si>
+    <t>ts1117</t>
+  </si>
+  <si>
+    <t>ts1307</t>
+  </si>
+  <si>
+    <t>ts1314</t>
+  </si>
+  <si>
+    <t>ts1323</t>
+  </si>
+  <si>
+    <t>ts1392</t>
+  </si>
+  <si>
+    <t>ts1434</t>
+  </si>
+  <si>
+    <t>ts1486</t>
+  </si>
+  <si>
+    <t>ts1519</t>
+  </si>
+  <si>
+    <t>ts1548</t>
+  </si>
+  <si>
+    <t>ts1567</t>
+  </si>
+  <si>
+    <t>ts1578</t>
+  </si>
+  <si>
+    <t>th1603</t>
+  </si>
+  <si>
+    <t>th1857</t>
+  </si>
+  <si>
+    <t>td2421</t>
+  </si>
+  <si>
+    <t>rn3464</t>
+  </si>
+  <si>
+    <t>rq5268</t>
+  </si>
+  <si>
+    <t>rq5276</t>
+  </si>
+  <si>
+    <t>rq5285</t>
+  </si>
+  <si>
+    <t>rq5297</t>
+  </si>
+  <si>
+    <t>pi6454</t>
+  </si>
+  <si>
+    <t>pi6468</t>
+  </si>
+  <si>
+    <t>pi6480</t>
+  </si>
+  <si>
+    <t>pi6501</t>
+  </si>
+  <si>
+    <t>pi6506</t>
+  </si>
+  <si>
+    <t>pi6600</t>
+  </si>
+  <si>
+    <t>pi6624</t>
+  </si>
+  <si>
+    <t>SOLD TIPS</t>
+  </si>
+  <si>
+    <t>ts1105</t>
+  </si>
+  <si>
+    <t>ts1308</t>
+  </si>
+  <si>
+    <t>ts1315</t>
+  </si>
+  <si>
+    <t>ts1324</t>
+  </si>
+  <si>
+    <t>ts1393</t>
+  </si>
+  <si>
+    <t>ts1441</t>
+  </si>
+  <si>
+    <t>ts1515</t>
+  </si>
+  <si>
+    <t>ts1520</t>
+  </si>
+  <si>
+    <t>ts1555</t>
+  </si>
+  <si>
+    <t>ts1575</t>
+  </si>
+  <si>
+    <t>ts1622</t>
+  </si>
+  <si>
+    <t>td2422</t>
+  </si>
+  <si>
+    <t>rn3466</t>
+  </si>
+  <si>
+    <t>rq5271</t>
+  </si>
+  <si>
+    <t>rq5277</t>
+  </si>
+  <si>
+    <t>rq5287</t>
+  </si>
+  <si>
+    <t>rq5298</t>
+  </si>
+  <si>
+    <t>pi6456</t>
+  </si>
+  <si>
+    <t>pi6466</t>
+  </si>
+  <si>
+    <t>pi6483</t>
+  </si>
+  <si>
+    <t>pi6502</t>
+  </si>
+  <si>
+    <t>pi6507</t>
+  </si>
+  <si>
+    <t>pi6602</t>
+  </si>
+  <si>
+    <t>pi6626</t>
+  </si>
+  <si>
+    <t>ts1104</t>
+  </si>
+  <si>
+    <t>ts1301</t>
+  </si>
+  <si>
+    <t>ts1311</t>
+  </si>
+  <si>
+    <t>ts1316</t>
+  </si>
+  <si>
+    <t>ts1325</t>
+  </si>
+  <si>
+    <t>ts1442</t>
+  </si>
+  <si>
+    <t>ts1516</t>
+  </si>
+  <si>
+    <t>ts1542</t>
+  </si>
+  <si>
+    <t>ts1556</t>
+  </si>
+  <si>
+    <t>ts1576</t>
+  </si>
+  <si>
+    <t>ts1586</t>
+  </si>
+  <si>
+    <t>ts1642</t>
+  </si>
+  <si>
+    <t>th1861</t>
+  </si>
+  <si>
+    <t>td2469</t>
+  </si>
+  <si>
+    <t>GAS ARRESTS</t>
+  </si>
+  <si>
+    <t>rs5615</t>
+  </si>
+  <si>
+    <t>sl2635</t>
+  </si>
+  <si>
+    <t>sl2670</t>
+  </si>
+  <si>
+    <t>sl2680</t>
+  </si>
+  <si>
+    <t>sl2636</t>
+  </si>
+  <si>
+    <t>LED LENSES</t>
+  </si>
+  <si>
+    <t>mm2520</t>
+  </si>
+  <si>
+    <t>mm1900</t>
+  </si>
+  <si>
+    <t>GLASS SWITCHES</t>
+  </si>
+  <si>
+    <t>PELTIERS</t>
+  </si>
+  <si>
+    <t>MIC INSERTS</t>
+  </si>
+  <si>
+    <t>AO5550</t>
+  </si>
+  <si>
+    <t>ZM9904</t>
+  </si>
+  <si>
+    <t>PM0854</t>
+  </si>
+  <si>
+    <t>QC3599</t>
+  </si>
+  <si>
+    <t>TD2410</t>
+  </si>
+  <si>
+    <t>3D PRINTER PARTS</t>
+  </si>
+  <si>
+    <t>rs5422</t>
+  </si>
+  <si>
+    <t>st3375</t>
+  </si>
+  <si>
+    <t>sl2671</t>
+  </si>
+  <si>
+    <t>sl2681</t>
+  </si>
+  <si>
+    <t>sl2690</t>
+  </si>
+  <si>
+    <t>mm2532</t>
+  </si>
+  <si>
+    <t>SM1035</t>
+  </si>
+  <si>
+    <t>ZP9100</t>
+  </si>
+  <si>
+    <t>AM4010</t>
+  </si>
+  <si>
+    <t>HH8610</t>
+  </si>
+  <si>
+    <t>QC8024</t>
+  </si>
+  <si>
+    <t>QM7450</t>
+  </si>
+  <si>
+    <t>QC8717</t>
+  </si>
+  <si>
+    <t>TL4320</t>
+  </si>
+  <si>
+    <t>rs5424</t>
+  </si>
+  <si>
+    <t>sl2673</t>
+  </si>
+  <si>
+    <t>sl2683</t>
+  </si>
+  <si>
+    <t>sl2692</t>
+  </si>
+  <si>
+    <t>mm2534</t>
+  </si>
+  <si>
+    <t>SM1002</t>
+  </si>
+  <si>
+    <t>ZP9102</t>
+  </si>
+  <si>
+    <t>AM4011</t>
+  </si>
+  <si>
+    <t>TL4277</t>
+  </si>
+  <si>
+    <t>rs5426</t>
+  </si>
+  <si>
+    <t>sl2674</t>
+  </si>
+  <si>
+    <t>sl2684</t>
+  </si>
+  <si>
+    <t>sl2695</t>
+  </si>
+  <si>
+    <t>ZP9104</t>
+  </si>
+  <si>
+    <t>TL4278</t>
+  </si>
+  <si>
+    <t>rs5610</t>
+  </si>
+  <si>
+    <t>sl2675</t>
+  </si>
+  <si>
+    <t>sl2685</t>
+  </si>
+  <si>
+    <t>sl2696</t>
+  </si>
+  <si>
+    <t>z8826</t>
+  </si>
+  <si>
+    <t>TL4284</t>
   </si>
 </sst>
 </file>
@@ -2263,10 +3028,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -2306,16 +3071,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2328,8 +3093,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2352,18 +3133,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2377,9 +3158,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2391,24 +3172,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2454,13 +3219,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2472,67 +3231,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2550,13 +3255,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2568,7 +3339,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2580,13 +3363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2598,19 +3375,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2687,6 +3452,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2710,21 +3486,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2742,73 +3507,73 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2817,67 +3582,69 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="10" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="23" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="30" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3199,28 +3966,37 @@
   <sheetPr/>
   <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="3.57142857142857" customWidth="1"/>
+    <col min="2" max="2" width="13.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="11.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="7.85714285714286" customWidth="1"/>
+    <col min="4" max="4" width="8.14285714285714" customWidth="1"/>
+    <col min="5" max="7" width="7.85714285714286" customWidth="1"/>
     <col min="8" max="9" width="12.1428571428571" customWidth="1"/>
+    <col min="10" max="10" width="13.1428571428571" customWidth="1"/>
     <col min="11" max="11" width="11.5714285714286" customWidth="1"/>
-    <col min="12" max="12" width="14.1428571428571" customWidth="1"/>
-    <col min="16" max="16" width="7.85714285714286" customWidth="1"/>
+    <col min="12" max="12" width="15.5714285714286" customWidth="1"/>
+    <col min="13" max="13" width="7.85714285714286" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="10.2857142857143" customWidth="1"/>
+    <col min="16" max="16" width="12.8571428571429" customWidth="1"/>
+    <col min="17" max="17" width="8.28571428571429" customWidth="1"/>
     <col min="18" max="18" width="10.8571428571429" customWidth="1"/>
     <col min="19" max="19" width="12.1428571428571" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
     <col min="21" max="21" width="12.4285714285714" customWidth="1"/>
+    <col min="22" max="22" width="7.85714285714286" customWidth="1"/>
     <col min="23" max="23" width="8.14285714285714" customWidth="1"/>
     <col min="24" max="24" width="7.85714285714286" customWidth="1"/>
     <col min="25" max="25" width="13.8571428571429" customWidth="1"/>
-    <col min="26" max="26" width="7.85714285714286" customWidth="1"/>
+    <col min="26" max="26" width="8.71428571428571" customWidth="1"/>
     <col min="27" max="27" width="9.85714285714286" customWidth="1"/>
-    <col min="28" max="28" width="8.85714285714286" customWidth="1"/>
+    <col min="28" max="28" width="18.7142857142857" customWidth="1"/>
     <col min="29" max="29" width="15.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5000,7 +5776,7 @@
       <c r="D23" t="s">
         <v>493</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="1" t="s">
         <v>494</v>
       </c>
       <c r="F23" t="s">
@@ -5030,7 +5806,7 @@
       <c r="N23" t="s">
         <v>503</v>
       </c>
-      <c r="O23" s="7" t="s">
+      <c r="O23" s="3" t="s">
         <v>504</v>
       </c>
       <c r="P23" t="s">
@@ -5086,10 +5862,10 @@
       <c r="C24" t="s">
         <v>520</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="1" t="s">
         <v>522</v>
       </c>
       <c r="F24" t="s">
@@ -5693,48 +6469,66 @@
       <c r="H32" t="s">
         <v>691</v>
       </c>
+      <c r="I32" t="s">
+        <v>692</v>
+      </c>
       <c r="J32" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="K32" t="s">
-        <v>693</v>
-      </c>
-      <c r="L32" s="7" t="s">
         <v>694</v>
       </c>
+      <c r="L32" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="M32" t="s">
+        <v>696</v>
+      </c>
+      <c r="N32" t="s">
+        <v>697</v>
+      </c>
       <c r="O32" t="s">
-        <v>695</v>
+        <v>698</v>
+      </c>
+      <c r="P32" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>700</v>
       </c>
       <c r="R32" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
       <c r="S32" t="s">
-        <v>697</v>
-      </c>
-      <c r="T32" s="7" t="s">
-        <v>698</v>
+        <v>702</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>703</v>
       </c>
       <c r="U32" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="V32" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
       <c r="W32" t="s">
-        <v>701</v>
+        <v>706</v>
       </c>
       <c r="X32" s="5"/>
       <c r="Y32" t="s">
-        <v>702</v>
-      </c>
-      <c r="Z32" s="7" t="s">
-        <v>703</v>
+        <v>707</v>
+      </c>
+      <c r="Z32" s="3" t="s">
+        <v>708</v>
       </c>
       <c r="AA32" t="s">
-        <v>704</v>
+        <v>709</v>
+      </c>
+      <c r="AB32" s="6" t="s">
+        <v>710</v>
       </c>
       <c r="AC32" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
     </row>
     <row r="33" spans="1:29">
@@ -5742,120 +6536,344 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="C33" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="D33" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="E33" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="F33" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="G33" t="s">
-        <v>711</v>
+        <v>717</v>
+      </c>
+      <c r="H33" t="s">
+        <v>718</v>
+      </c>
+      <c r="I33" t="s">
+        <v>719</v>
+      </c>
+      <c r="J33" t="s">
+        <v>720</v>
+      </c>
+      <c r="K33" t="s">
+        <v>721</v>
+      </c>
+      <c r="L33" t="s">
+        <v>722</v>
+      </c>
+      <c r="M33" t="s">
+        <v>723</v>
+      </c>
+      <c r="N33" t="s">
+        <v>724</v>
+      </c>
+      <c r="O33" t="s">
+        <v>725</v>
+      </c>
+      <c r="P33" t="s">
+        <v>726</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>727</v>
+      </c>
+      <c r="R33" t="s">
+        <v>728</v>
+      </c>
+      <c r="S33" t="s">
+        <v>729</v>
       </c>
       <c r="T33" t="s">
-        <v>712</v>
+        <v>730</v>
       </c>
       <c r="U33" t="s">
-        <v>713</v>
+        <v>731</v>
+      </c>
+      <c r="V33" t="s">
+        <v>732</v>
       </c>
       <c r="W33" t="s">
-        <v>714</v>
+        <v>733</v>
       </c>
       <c r="X33" t="s">
-        <v>715</v>
+        <v>734</v>
       </c>
       <c r="Y33" t="s">
-        <v>716</v>
+        <v>735</v>
       </c>
       <c r="Z33" t="s">
-        <v>717</v>
+        <v>736</v>
       </c>
       <c r="AA33" t="s">
-        <v>718</v>
+        <v>737</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>738</v>
       </c>
       <c r="AC33" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:29">
       <c r="A34" s="2">
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>720</v>
+        <v>740</v>
       </c>
       <c r="C34" t="s">
-        <v>721</v>
+        <v>741</v>
       </c>
       <c r="D34" t="s">
-        <v>722</v>
+        <v>742</v>
       </c>
       <c r="E34" t="s">
-        <v>723</v>
+        <v>743</v>
       </c>
       <c r="F34" t="s">
-        <v>724</v>
+        <v>744</v>
       </c>
       <c r="G34" t="s">
-        <v>725</v>
+        <v>745</v>
+      </c>
+      <c r="H34" t="s">
+        <v>746</v>
+      </c>
+      <c r="I34" t="s">
+        <v>747</v>
+      </c>
+      <c r="J34" t="s">
+        <v>748</v>
+      </c>
+      <c r="K34" s="7"/>
+      <c r="L34" t="s">
+        <v>749</v>
+      </c>
+      <c r="M34" t="s">
+        <v>750</v>
+      </c>
+      <c r="N34" t="s">
+        <v>751</v>
+      </c>
+      <c r="O34" t="s">
+        <v>752</v>
+      </c>
+      <c r="P34" t="s">
+        <v>753</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>754</v>
+      </c>
+      <c r="R34" t="s">
+        <v>755</v>
+      </c>
+      <c r="S34" t="s">
+        <v>756</v>
       </c>
       <c r="T34" t="s">
-        <v>726</v>
+        <v>757</v>
       </c>
       <c r="U34" t="s">
-        <v>727</v>
+        <v>758</v>
+      </c>
+      <c r="V34" t="s">
+        <v>759</v>
+      </c>
+      <c r="W34" t="s">
+        <v>760</v>
+      </c>
+      <c r="X34" t="s">
+        <v>761</v>
+      </c>
+      <c r="Y34" s="6" t="s">
+        <v>762</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>763</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>764</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>765</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>766</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:29">
       <c r="A35" s="2">
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>728</v>
+        <v>767</v>
       </c>
       <c r="C35" t="s">
-        <v>729</v>
+        <v>768</v>
       </c>
       <c r="D35" t="s">
-        <v>730</v>
+        <v>769</v>
       </c>
       <c r="E35" t="s">
-        <v>731</v>
+        <v>770</v>
       </c>
       <c r="F35" t="s">
-        <v>732</v>
+        <v>771</v>
       </c>
       <c r="G35" t="s">
-        <v>733</v>
+        <v>772</v>
+      </c>
+      <c r="H35" t="s">
+        <v>773</v>
+      </c>
+      <c r="I35" t="s">
+        <v>774</v>
+      </c>
+      <c r="J35" t="s">
+        <v>775</v>
+      </c>
+      <c r="K35" s="7"/>
+      <c r="L35" t="s">
+        <v>776</v>
+      </c>
+      <c r="M35" t="s">
+        <v>777</v>
+      </c>
+      <c r="N35" t="s">
+        <v>778</v>
+      </c>
+      <c r="O35" t="s">
+        <v>779</v>
+      </c>
+      <c r="P35" t="s">
+        <v>780</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>781</v>
+      </c>
+      <c r="R35" t="s">
+        <v>782</v>
+      </c>
+      <c r="S35" t="s">
+        <v>783</v>
+      </c>
+      <c r="T35" t="s">
+        <v>784</v>
+      </c>
+      <c r="U35" t="s">
+        <v>785</v>
+      </c>
+      <c r="V35" t="s">
+        <v>786</v>
+      </c>
+      <c r="W35" s="7"/>
+      <c r="X35" t="s">
+        <v>787</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>788</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>789</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>790</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>791</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>792</v>
       </c>
     </row>
-    <row r="36" ht="15.75" spans="1:7">
+    <row r="36" ht="15.75" spans="1:29">
       <c r="A36" s="2">
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>734</v>
+        <v>793</v>
       </c>
       <c r="C36" t="s">
-        <v>735</v>
+        <v>794</v>
       </c>
       <c r="D36" t="s">
-        <v>736</v>
+        <v>795</v>
       </c>
       <c r="E36" t="s">
-        <v>737</v>
+        <v>796</v>
       </c>
       <c r="F36" t="s">
-        <v>738</v>
+        <v>797</v>
       </c>
       <c r="G36" s="5"/>
+      <c r="H36" t="s">
+        <v>798</v>
+      </c>
+      <c r="I36" t="s">
+        <v>799</v>
+      </c>
+      <c r="J36" t="s">
+        <v>800</v>
+      </c>
+      <c r="K36" s="7"/>
+      <c r="L36" t="s">
+        <v>801</v>
+      </c>
+      <c r="M36" t="s">
+        <v>802</v>
+      </c>
+      <c r="N36" t="s">
+        <v>803</v>
+      </c>
+      <c r="O36" t="s">
+        <v>804</v>
+      </c>
+      <c r="P36" t="s">
+        <v>805</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>806</v>
+      </c>
+      <c r="R36" t="s">
+        <v>807</v>
+      </c>
+      <c r="S36" t="s">
+        <v>808</v>
+      </c>
+      <c r="T36" t="s">
+        <v>809</v>
+      </c>
+      <c r="U36" t="s">
+        <v>810</v>
+      </c>
+      <c r="V36" t="s">
+        <v>811</v>
+      </c>
+      <c r="W36" s="7"/>
+      <c r="X36" t="s">
+        <v>812</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>813</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>814</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>815</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>816</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="37" ht="4" customHeight="1" spans="1:29">
       <c r="A37" s="4"/>
@@ -5888,53 +6906,437 @@
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
     </row>
-    <row r="38" ht="15.75" spans="1:8">
+    <row r="38" ht="15.75" spans="1:29">
       <c r="A38" s="2">
         <v>31</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>739</v>
+      <c r="B38" s="3" t="s">
+        <v>818</v>
       </c>
       <c r="C38" t="s">
-        <v>740</v>
+        <v>819</v>
       </c>
       <c r="D38" t="s">
-        <v>741</v>
+        <v>820</v>
       </c>
       <c r="E38" t="s">
-        <v>742</v>
+        <v>821</v>
       </c>
       <c r="F38" t="s">
-        <v>743</v>
+        <v>822</v>
       </c>
       <c r="G38" t="s">
-        <v>744</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>745</v>
+        <v>823</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="I38" t="s">
+        <v>825</v>
+      </c>
+      <c r="J38" t="s">
+        <v>826</v>
+      </c>
+      <c r="K38" t="s">
+        <v>827</v>
+      </c>
+      <c r="L38" t="s">
+        <v>828</v>
+      </c>
+      <c r="M38" t="s">
+        <v>829</v>
+      </c>
+      <c r="N38" t="s">
+        <v>830</v>
+      </c>
+      <c r="O38" t="s">
+        <v>831</v>
+      </c>
+      <c r="P38" t="s">
+        <v>832</v>
+      </c>
+      <c r="Q38" s="7"/>
+      <c r="R38" t="s">
+        <v>833</v>
+      </c>
+      <c r="S38" t="s">
+        <v>834</v>
+      </c>
+      <c r="T38" t="s">
+        <v>835</v>
+      </c>
+      <c r="U38" t="s">
+        <v>836</v>
+      </c>
+      <c r="V38" t="s">
+        <v>837</v>
+      </c>
+      <c r="W38" s="7"/>
+      <c r="X38" t="s">
+        <v>838</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>839</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>840</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>841</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>842</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>843</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:29">
       <c r="A39" s="2">
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>746</v>
+        <v>844</v>
+      </c>
+      <c r="C39" t="s">
+        <v>845</v>
+      </c>
+      <c r="D39" t="s">
+        <v>846</v>
+      </c>
+      <c r="E39" t="s">
+        <v>847</v>
+      </c>
+      <c r="F39" t="s">
+        <v>848</v>
+      </c>
+      <c r="G39" t="s">
+        <v>849</v>
+      </c>
+      <c r="H39" t="s">
+        <v>850</v>
+      </c>
+      <c r="I39" t="s">
+        <v>851</v>
+      </c>
+      <c r="J39" t="s">
+        <v>852</v>
+      </c>
+      <c r="K39" t="s">
+        <v>853</v>
+      </c>
+      <c r="L39" t="s">
+        <v>854</v>
+      </c>
+      <c r="M39" t="s">
+        <v>855</v>
+      </c>
+      <c r="N39" t="s">
+        <v>856</v>
+      </c>
+      <c r="O39" t="s">
+        <v>857</v>
+      </c>
+      <c r="P39" t="s">
+        <v>858</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>859</v>
+      </c>
+      <c r="R39" t="s">
+        <v>860</v>
+      </c>
+      <c r="S39" t="s">
+        <v>861</v>
+      </c>
+      <c r="T39" t="s">
+        <v>862</v>
+      </c>
+      <c r="U39" t="s">
+        <v>863</v>
+      </c>
+      <c r="V39" t="s">
+        <v>864</v>
+      </c>
+      <c r="W39" t="s">
+        <v>865</v>
+      </c>
+      <c r="X39" t="s">
+        <v>866</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>867</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>840</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>868</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>869</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>870</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:29">
       <c r="A40" s="2">
         <v>33</v>
       </c>
+      <c r="B40" t="s">
+        <v>871</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>872</v>
+      </c>
+      <c r="D40" t="s">
+        <v>873</v>
+      </c>
+      <c r="E40" t="s">
+        <v>874</v>
+      </c>
+      <c r="F40" t="s">
+        <v>875</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" t="s">
+        <v>876</v>
+      </c>
+      <c r="I40" t="s">
+        <v>877</v>
+      </c>
+      <c r="J40" t="s">
+        <v>878</v>
+      </c>
+      <c r="K40" t="s">
+        <v>879</v>
+      </c>
+      <c r="L40" t="s">
+        <v>880</v>
+      </c>
+      <c r="M40" t="s">
+        <v>881</v>
+      </c>
+      <c r="N40" t="s">
+        <v>882</v>
+      </c>
+      <c r="O40" t="s">
+        <v>883</v>
+      </c>
+      <c r="P40" t="s">
+        <v>884</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>885</v>
+      </c>
+      <c r="R40" t="s">
+        <v>886</v>
+      </c>
+      <c r="S40" t="s">
+        <v>887</v>
+      </c>
+      <c r="T40" t="s">
+        <v>888</v>
+      </c>
+      <c r="U40" t="s">
+        <v>889</v>
+      </c>
+      <c r="V40" t="s">
+        <v>890</v>
+      </c>
+      <c r="W40" t="s">
+        <v>891</v>
+      </c>
+      <c r="X40" t="s">
+        <v>892</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>893</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>894</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>895</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>896</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>897</v>
+      </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:29">
       <c r="A41" s="2">
         <v>34</v>
       </c>
+      <c r="B41" t="s">
+        <v>898</v>
+      </c>
+      <c r="C41" t="s">
+        <v>899</v>
+      </c>
+      <c r="D41" t="s">
+        <v>900</v>
+      </c>
+      <c r="E41" t="s">
+        <v>901</v>
+      </c>
+      <c r="F41" t="s">
+        <v>902</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" t="s">
+        <v>903</v>
+      </c>
+      <c r="I41" t="s">
+        <v>904</v>
+      </c>
+      <c r="J41" t="s">
+        <v>905</v>
+      </c>
+      <c r="K41" t="s">
+        <v>906</v>
+      </c>
+      <c r="L41" t="s">
+        <v>907</v>
+      </c>
+      <c r="M41" t="s">
+        <v>908</v>
+      </c>
+      <c r="N41" t="s">
+        <v>909</v>
+      </c>
+      <c r="O41" s="6" t="s">
+        <v>910</v>
+      </c>
+      <c r="P41" t="s">
+        <v>911</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>912</v>
+      </c>
+      <c r="R41" t="s">
+        <v>913</v>
+      </c>
+      <c r="S41" t="s">
+        <v>914</v>
+      </c>
+      <c r="T41" t="s">
+        <v>915</v>
+      </c>
+      <c r="U41" t="s">
+        <v>916</v>
+      </c>
+      <c r="V41" t="s">
+        <v>917</v>
+      </c>
+      <c r="W41" t="s">
+        <v>918</v>
+      </c>
+      <c r="X41" t="s">
+        <v>919</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>920</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>894</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>921</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>896</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>922</v>
+      </c>
     </row>
-    <row r="42" ht="15.75" spans="1:1">
+    <row r="42" ht="15.75" spans="1:29">
       <c r="A42" s="2">
         <v>35</v>
+      </c>
+      <c r="B42" t="s">
+        <v>923</v>
+      </c>
+      <c r="C42" t="s">
+        <v>924</v>
+      </c>
+      <c r="D42" t="s">
+        <v>925</v>
+      </c>
+      <c r="E42" t="s">
+        <v>926</v>
+      </c>
+      <c r="F42" t="s">
+        <v>927</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" t="s">
+        <v>928</v>
+      </c>
+      <c r="I42" t="s">
+        <v>929</v>
+      </c>
+      <c r="J42" t="s">
+        <v>930</v>
+      </c>
+      <c r="K42" t="s">
+        <v>931</v>
+      </c>
+      <c r="L42" t="s">
+        <v>932</v>
+      </c>
+      <c r="M42" t="s">
+        <v>933</v>
+      </c>
+      <c r="N42" t="s">
+        <v>934</v>
+      </c>
+      <c r="O42" t="s">
+        <v>935</v>
+      </c>
+      <c r="P42" t="s">
+        <v>936</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>937</v>
+      </c>
+      <c r="R42" t="s">
+        <v>938</v>
+      </c>
+      <c r="S42" t="s">
+        <v>939</v>
+      </c>
+      <c r="T42" s="7"/>
+      <c r="U42" t="s">
+        <v>940</v>
+      </c>
+      <c r="V42" t="s">
+        <v>941</v>
+      </c>
+      <c r="W42" t="s">
+        <v>942</v>
+      </c>
+      <c r="X42" t="s">
+        <v>943</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>944</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>945</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>946</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>947</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>948</v>
       </c>
     </row>
     <row r="43" ht="4" customHeight="1" spans="1:29">
@@ -5968,30 +7370,282 @@
       <c r="AB43" s="4"/>
       <c r="AC43" s="4"/>
     </row>
-    <row r="44" ht="15.75" spans="1:1">
+    <row r="44" ht="15.75" spans="1:29">
       <c r="A44" s="2">
         <v>36</v>
       </c>
+      <c r="B44" s="6" t="s">
+        <v>949</v>
+      </c>
+      <c r="C44" t="s">
+        <v>950</v>
+      </c>
+      <c r="D44" t="s">
+        <v>951</v>
+      </c>
+      <c r="E44" t="s">
+        <v>952</v>
+      </c>
+      <c r="F44" t="s">
+        <v>953</v>
+      </c>
+      <c r="G44" t="s">
+        <v>954</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>955</v>
+      </c>
+      <c r="I44" t="s">
+        <v>956</v>
+      </c>
+      <c r="J44" t="s">
+        <v>957</v>
+      </c>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="6" t="s">
+        <v>958</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>961</v>
+      </c>
+      <c r="R44" t="s">
+        <v>962</v>
+      </c>
+      <c r="S44" t="s">
+        <v>962</v>
+      </c>
+      <c r="T44" t="s">
+        <v>963</v>
+      </c>
+      <c r="U44" t="s">
+        <v>964</v>
+      </c>
+      <c r="V44" s="8"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="7"/>
+      <c r="Y44" s="7"/>
+      <c r="Z44" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="AA44" s="7"/>
+      <c r="AB44" s="6" t="s">
+        <v>966</v>
+      </c>
+      <c r="AC44" s="7"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:29">
       <c r="A45" s="2">
         <v>37</v>
       </c>
+      <c r="B45" t="s">
+        <v>967</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" t="s">
+        <v>968</v>
+      </c>
+      <c r="E45" t="s">
+        <v>969</v>
+      </c>
+      <c r="F45" t="s">
+        <v>970</v>
+      </c>
+      <c r="G45" t="s">
+        <v>971</v>
+      </c>
+      <c r="H45" s="7"/>
+      <c r="I45" t="s">
+        <v>972</v>
+      </c>
+      <c r="J45" t="s">
+        <v>957</v>
+      </c>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" t="s">
+        <v>973</v>
+      </c>
+      <c r="O45" t="s">
+        <v>974</v>
+      </c>
+      <c r="P45" t="s">
+        <v>975</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>976</v>
+      </c>
+      <c r="R45" t="s">
+        <v>977</v>
+      </c>
+      <c r="S45" s="8"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="9" t="s">
+        <v>978</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>979</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>980</v>
+      </c>
+      <c r="AC45" s="7"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:29">
       <c r="A46" s="2">
         <v>38</v>
       </c>
+      <c r="B46" t="s">
+        <v>981</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" t="s">
+        <v>982</v>
+      </c>
+      <c r="F46" t="s">
+        <v>983</v>
+      </c>
+      <c r="G46" t="s">
+        <v>984</v>
+      </c>
+      <c r="H46" s="7"/>
+      <c r="I46" t="s">
+        <v>985</v>
+      </c>
+      <c r="J46" t="s">
+        <v>957</v>
+      </c>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" t="s">
+        <v>986</v>
+      </c>
+      <c r="O46" t="s">
+        <v>987</v>
+      </c>
+      <c r="P46" t="s">
+        <v>988</v>
+      </c>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="7"/>
+      <c r="AB46" t="s">
+        <v>989</v>
+      </c>
+      <c r="AC46" s="7"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:29">
       <c r="A47" s="2">
         <v>39</v>
       </c>
+      <c r="B47" t="s">
+        <v>990</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" t="s">
+        <v>991</v>
+      </c>
+      <c r="F47" t="s">
+        <v>992</v>
+      </c>
+      <c r="G47" t="s">
+        <v>993</v>
+      </c>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" t="s">
+        <v>994</v>
+      </c>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+      <c r="AA47" s="7"/>
+      <c r="AB47" t="s">
+        <v>995</v>
+      </c>
+      <c r="AC47" s="7"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:29">
       <c r="A48" s="2">
         <v>40</v>
       </c>
+      <c r="B48" t="s">
+        <v>996</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" t="s">
+        <v>997</v>
+      </c>
+      <c r="F48" t="s">
+        <v>998</v>
+      </c>
+      <c r="G48" t="s">
+        <v>999</v>
+      </c>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="7"/>
+      <c r="AB48" t="s">
+        <v>1001</v>
+      </c>
+      <c r="AC48" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>